<commit_message>
new version of IG
</commit_message>
<xml_diff>
--- a/CodeSystem-airport-code-system.xlsx
+++ b/CodeSystem-airport-code-system.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://example.org/CodeSystem/airport-code-system</t>
+    <t>http://hl7.org/fhir/us/reportofilltraveler/CodeSystem/airport-code-system</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-28T21:37:28-05:00</t>
+    <t>2023-12-05T13:08:56-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>